<commit_message>
revert conversion of U -> T
</commit_message>
<xml_diff>
--- a/SupplementaryTable1.xlsx
+++ b/SupplementaryTable1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sonia Ling\Desktop\calculate_dr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41732DD1-DB83-4DB8-A8CE-E221D131077B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBACFEE0-BD1E-4C71-941A-FDDC0BF75970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10260" xr2:uid="{E845C743-C63C-FC46-A70F-BF0704E39555}"/>
   </bookViews>
@@ -49,772 +49,772 @@
     <t>fit_R</t>
   </si>
   <si>
-    <t>AAUAA</t>
-  </si>
-  <si>
-    <t>AAUAC</t>
-  </si>
-  <si>
-    <t>AAUAG</t>
-  </si>
-  <si>
-    <t>AAUAU</t>
-  </si>
-  <si>
-    <t>AAUCA</t>
-  </si>
-  <si>
-    <t>AAUCC</t>
-  </si>
-  <si>
-    <t>AAUCG</t>
-  </si>
-  <si>
-    <t>AAUCU</t>
-  </si>
-  <si>
-    <t>AAUGA</t>
-  </si>
-  <si>
-    <t>AAUGC</t>
-  </si>
-  <si>
-    <t>AAUGG</t>
-  </si>
-  <si>
-    <t>AAUGU</t>
-  </si>
-  <si>
-    <t>AAUUA</t>
-  </si>
-  <si>
-    <t>AAUUC</t>
-  </si>
-  <si>
-    <t>AAUUG</t>
-  </si>
-  <si>
-    <t>AAUUU</t>
-  </si>
-  <si>
-    <t>ACUAA</t>
-  </si>
-  <si>
-    <t>ACUAC</t>
-  </si>
-  <si>
-    <t>ACUAG</t>
-  </si>
-  <si>
-    <t>ACUAU</t>
-  </si>
-  <si>
-    <t>ACUCA</t>
-  </si>
-  <si>
-    <t>ACUCC</t>
-  </si>
-  <si>
-    <t>ACUCG</t>
-  </si>
-  <si>
-    <t>ACUCU</t>
-  </si>
-  <si>
-    <t>ACUGA</t>
-  </si>
-  <si>
-    <t>ACUGC</t>
-  </si>
-  <si>
-    <t>ACUGG</t>
-  </si>
-  <si>
-    <t>ACUGU</t>
-  </si>
-  <si>
-    <t>ACUUA</t>
-  </si>
-  <si>
-    <t>ACUUC</t>
-  </si>
-  <si>
-    <t>ACUUG</t>
-  </si>
-  <si>
-    <t>ACUUU</t>
-  </si>
-  <si>
-    <t>AGUAA</t>
-  </si>
-  <si>
-    <t>AGUAC</t>
-  </si>
-  <si>
-    <t>AGUAG</t>
-  </si>
-  <si>
-    <t>AGUAU</t>
-  </si>
-  <si>
-    <t>AGUCA</t>
-  </si>
-  <si>
-    <t>AGUCC</t>
-  </si>
-  <si>
-    <t>AGUCG</t>
-  </si>
-  <si>
-    <t>AGUCU</t>
-  </si>
-  <si>
-    <t>AGUGA</t>
-  </si>
-  <si>
-    <t>AGUGC</t>
-  </si>
-  <si>
-    <t>AGUGG</t>
-  </si>
-  <si>
-    <t>AGUGU</t>
-  </si>
-  <si>
-    <t>AGUUA</t>
-  </si>
-  <si>
-    <t>AGUUC</t>
-  </si>
-  <si>
-    <t>AGUUG</t>
-  </si>
-  <si>
-    <t>AGUUU</t>
-  </si>
-  <si>
-    <t>AUUAA</t>
-  </si>
-  <si>
-    <t>AUUAC</t>
-  </si>
-  <si>
-    <t>AUUAG</t>
-  </si>
-  <si>
-    <t>AUUAU</t>
-  </si>
-  <si>
-    <t>AUUCA</t>
-  </si>
-  <si>
-    <t>AUUCC</t>
-  </si>
-  <si>
-    <t>AUUCG</t>
-  </si>
-  <si>
-    <t>AUUCU</t>
-  </si>
-  <si>
-    <t>AUUGA</t>
-  </si>
-  <si>
-    <t>AUUGC</t>
-  </si>
-  <si>
-    <t>AUUGG</t>
-  </si>
-  <si>
-    <t>AUUGU</t>
-  </si>
-  <si>
-    <t>AUUUA</t>
-  </si>
-  <si>
-    <t>AUUUC</t>
-  </si>
-  <si>
-    <t>AUUUG</t>
-  </si>
-  <si>
-    <t>AUUUU</t>
-  </si>
-  <si>
-    <t>CAUAA</t>
-  </si>
-  <si>
-    <t>CAUAC</t>
-  </si>
-  <si>
-    <t>CAUAG</t>
-  </si>
-  <si>
-    <t>CAUAU</t>
-  </si>
-  <si>
-    <t>CAUCA</t>
-  </si>
-  <si>
-    <t>CAUCC</t>
-  </si>
-  <si>
-    <t>CAUCG</t>
-  </si>
-  <si>
-    <t>CAUCU</t>
-  </si>
-  <si>
-    <t>CAUGA</t>
-  </si>
-  <si>
-    <t>CAUGC</t>
-  </si>
-  <si>
-    <t>CAUGG</t>
-  </si>
-  <si>
-    <t>CAUGU</t>
-  </si>
-  <si>
-    <t>CAUUA</t>
-  </si>
-  <si>
-    <t>CAUUC</t>
-  </si>
-  <si>
-    <t>CAUUG</t>
-  </si>
-  <si>
-    <t>CAUUU</t>
-  </si>
-  <si>
-    <t>CCUAA</t>
-  </si>
-  <si>
-    <t>CCUAC</t>
-  </si>
-  <si>
-    <t>CCUAG</t>
-  </si>
-  <si>
-    <t>CCUAU</t>
-  </si>
-  <si>
-    <t>CCUCA</t>
-  </si>
-  <si>
-    <t>CCUCC</t>
-  </si>
-  <si>
-    <t>CCUCG</t>
-  </si>
-  <si>
-    <t>CCUCU</t>
-  </si>
-  <si>
-    <t>CCUGA</t>
-  </si>
-  <si>
-    <t>CCUGC</t>
-  </si>
-  <si>
-    <t>CCUGG</t>
-  </si>
-  <si>
-    <t>CCUGU</t>
-  </si>
-  <si>
-    <t>CCUUA</t>
-  </si>
-  <si>
-    <t>CCUUC</t>
-  </si>
-  <si>
-    <t>CCUUG</t>
-  </si>
-  <si>
-    <t>CCUUU</t>
-  </si>
-  <si>
-    <t>CGUAA</t>
-  </si>
-  <si>
-    <t>CGUAC</t>
-  </si>
-  <si>
-    <t>CGUAG</t>
-  </si>
-  <si>
-    <t>CGUAU</t>
-  </si>
-  <si>
-    <t>CGUCA</t>
-  </si>
-  <si>
-    <t>CGUCC</t>
-  </si>
-  <si>
-    <t>CGUCG</t>
-  </si>
-  <si>
-    <t>CGUCU</t>
-  </si>
-  <si>
-    <t>CGUGA</t>
-  </si>
-  <si>
-    <t>CGUGC</t>
-  </si>
-  <si>
-    <t>CGUGG</t>
-  </si>
-  <si>
-    <t>CGUGU</t>
-  </si>
-  <si>
-    <t>CGUUA</t>
-  </si>
-  <si>
-    <t>CGUUC</t>
-  </si>
-  <si>
-    <t>CGUUG</t>
-  </si>
-  <si>
-    <t>CGUUU</t>
-  </si>
-  <si>
-    <t>CUUAA</t>
-  </si>
-  <si>
-    <t>CUUAC</t>
-  </si>
-  <si>
-    <t>CUUAG</t>
-  </si>
-  <si>
-    <t>CUUAU</t>
-  </si>
-  <si>
-    <t>CUUCA</t>
-  </si>
-  <si>
-    <t>CUUCC</t>
-  </si>
-  <si>
-    <t>CUUCG</t>
-  </si>
-  <si>
-    <t>CUUCU</t>
-  </si>
-  <si>
-    <t>CUUGA</t>
-  </si>
-  <si>
-    <t>CUUGC</t>
-  </si>
-  <si>
-    <t>CUUGG</t>
-  </si>
-  <si>
-    <t>CUUGU</t>
-  </si>
-  <si>
-    <t>CUUUA</t>
-  </si>
-  <si>
-    <t>CUUUC</t>
-  </si>
-  <si>
-    <t>CUUUG</t>
-  </si>
-  <si>
-    <t>CUUUU</t>
-  </si>
-  <si>
-    <t>GAUAA</t>
-  </si>
-  <si>
-    <t>GAUAC</t>
-  </si>
-  <si>
-    <t>GAUAG</t>
-  </si>
-  <si>
-    <t>GAUAU</t>
-  </si>
-  <si>
-    <t>GAUCA</t>
-  </si>
-  <si>
-    <t>GAUCC</t>
-  </si>
-  <si>
-    <t>GAUCG</t>
-  </si>
-  <si>
-    <t>GAUCU</t>
-  </si>
-  <si>
-    <t>GAUGA</t>
-  </si>
-  <si>
-    <t>GAUGC</t>
-  </si>
-  <si>
-    <t>GAUGG</t>
-  </si>
-  <si>
-    <t>GAUGU</t>
-  </si>
-  <si>
-    <t>GAUUA</t>
-  </si>
-  <si>
-    <t>GAUUC</t>
-  </si>
-  <si>
-    <t>GAUUG</t>
-  </si>
-  <si>
-    <t>GAUUU</t>
-  </si>
-  <si>
-    <t>GCUAA</t>
-  </si>
-  <si>
-    <t>GCUAC</t>
-  </si>
-  <si>
-    <t>GCUAG</t>
-  </si>
-  <si>
-    <t>GCUAU</t>
-  </si>
-  <si>
-    <t>GCUCA</t>
-  </si>
-  <si>
-    <t>GCUCC</t>
-  </si>
-  <si>
-    <t>GCUCG</t>
-  </si>
-  <si>
-    <t>GCUCU</t>
-  </si>
-  <si>
-    <t>GCUGA</t>
-  </si>
-  <si>
-    <t>GCUGC</t>
-  </si>
-  <si>
-    <t>GCUGG</t>
-  </si>
-  <si>
-    <t>GCUGU</t>
-  </si>
-  <si>
-    <t>GCUUA</t>
-  </si>
-  <si>
-    <t>GCUUC</t>
-  </si>
-  <si>
-    <t>GCUUG</t>
-  </si>
-  <si>
-    <t>GCUUU</t>
-  </si>
-  <si>
-    <t>GGUAA</t>
-  </si>
-  <si>
-    <t>GGUAC</t>
-  </si>
-  <si>
-    <t>GGUAG</t>
-  </si>
-  <si>
-    <t>GGUAU</t>
-  </si>
-  <si>
-    <t>GGUCA</t>
-  </si>
-  <si>
-    <t>GGUCC</t>
-  </si>
-  <si>
-    <t>GGUCG</t>
-  </si>
-  <si>
-    <t>GGUCU</t>
-  </si>
-  <si>
-    <t>GGUGA</t>
-  </si>
-  <si>
-    <t>GGUGC</t>
-  </si>
-  <si>
-    <t>GGUGG</t>
-  </si>
-  <si>
-    <t>GGUGU</t>
-  </si>
-  <si>
-    <t>GGUUA</t>
-  </si>
-  <si>
-    <t>GGUUC</t>
-  </si>
-  <si>
-    <t>GGUUG</t>
-  </si>
-  <si>
-    <t>GGUUU</t>
-  </si>
-  <si>
-    <t>GUUAA</t>
-  </si>
-  <si>
-    <t>GUUAC</t>
-  </si>
-  <si>
-    <t>GUUAG</t>
-  </si>
-  <si>
-    <t>GUUAU</t>
-  </si>
-  <si>
-    <t>GUUCA</t>
-  </si>
-  <si>
-    <t>GUUCC</t>
-  </si>
-  <si>
-    <t>GUUCG</t>
-  </si>
-  <si>
-    <t>GUUCU</t>
-  </si>
-  <si>
-    <t>GUUGA</t>
-  </si>
-  <si>
-    <t>GUUGC</t>
-  </si>
-  <si>
-    <t>GUUGG</t>
-  </si>
-  <si>
-    <t>GUUGU</t>
-  </si>
-  <si>
-    <t>GUUUA</t>
-  </si>
-  <si>
-    <t>GUUUC</t>
-  </si>
-  <si>
-    <t>GUUUG</t>
-  </si>
-  <si>
-    <t>GUUUU</t>
-  </si>
-  <si>
-    <t>UAUAA</t>
-  </si>
-  <si>
-    <t>UAUAC</t>
-  </si>
-  <si>
-    <t>UAUAG</t>
-  </si>
-  <si>
-    <t>UAUAU</t>
-  </si>
-  <si>
-    <t>UAUCA</t>
-  </si>
-  <si>
-    <t>UAUCC</t>
-  </si>
-  <si>
-    <t>UAUCG</t>
-  </si>
-  <si>
-    <t>UAUCU</t>
-  </si>
-  <si>
-    <t>UAUGA</t>
-  </si>
-  <si>
-    <t>UAUGC</t>
-  </si>
-  <si>
-    <t>UAUGG</t>
-  </si>
-  <si>
-    <t>UAUGU</t>
-  </si>
-  <si>
-    <t>UAUUA</t>
-  </si>
-  <si>
-    <t>UAUUC</t>
-  </si>
-  <si>
-    <t>UAUUG</t>
-  </si>
-  <si>
-    <t>UAUUU</t>
-  </si>
-  <si>
-    <t>UCUAA</t>
-  </si>
-  <si>
-    <t>UCUAC</t>
-  </si>
-  <si>
-    <t>UCUAG</t>
-  </si>
-  <si>
-    <t>UCUAU</t>
-  </si>
-  <si>
-    <t>UCUCA</t>
-  </si>
-  <si>
-    <t>UCUCC</t>
-  </si>
-  <si>
-    <t>UCUCG</t>
-  </si>
-  <si>
-    <t>UCUCU</t>
-  </si>
-  <si>
-    <t>UCUGA</t>
-  </si>
-  <si>
-    <t>UCUGC</t>
-  </si>
-  <si>
-    <t>UCUGG</t>
-  </si>
-  <si>
-    <t>UCUGU</t>
-  </si>
-  <si>
-    <t>UCUUA</t>
-  </si>
-  <si>
-    <t>UCUUC</t>
-  </si>
-  <si>
-    <t>UCUUG</t>
-  </si>
-  <si>
-    <t>UCUUU</t>
-  </si>
-  <si>
-    <t>UGUAA</t>
-  </si>
-  <si>
-    <t>UGUAC</t>
-  </si>
-  <si>
-    <t>UGUAG</t>
-  </si>
-  <si>
-    <t>UGUAU</t>
-  </si>
-  <si>
-    <t>UGUCA</t>
-  </si>
-  <si>
-    <t>UGUCC</t>
-  </si>
-  <si>
-    <t>UGUCG</t>
-  </si>
-  <si>
-    <t>UGUCU</t>
-  </si>
-  <si>
-    <t>UGUGA</t>
-  </si>
-  <si>
-    <t>UGUGC</t>
-  </si>
-  <si>
-    <t>UGUGG</t>
-  </si>
-  <si>
-    <t>UGUGU</t>
-  </si>
-  <si>
-    <t>UGUUA</t>
-  </si>
-  <si>
-    <t>UGUUC</t>
-  </si>
-  <si>
-    <t>UGUUG</t>
-  </si>
-  <si>
-    <t>UGUUU</t>
-  </si>
-  <si>
-    <t>UUUAA</t>
-  </si>
-  <si>
-    <t>UUUAC</t>
-  </si>
-  <si>
-    <t>UUUAG</t>
-  </si>
-  <si>
-    <t>UUUAU</t>
-  </si>
-  <si>
-    <t>UUUCA</t>
-  </si>
-  <si>
-    <t>UUUCC</t>
-  </si>
-  <si>
-    <t>UUUCG</t>
-  </si>
-  <si>
-    <t>UUUCU</t>
-  </si>
-  <si>
-    <t>UUUGA</t>
-  </si>
-  <si>
-    <t>UUUGC</t>
-  </si>
-  <si>
-    <t>UUUGG</t>
-  </si>
-  <si>
-    <t>UUUGU</t>
-  </si>
-  <si>
-    <t>UUUUA</t>
-  </si>
-  <si>
-    <t>UUUUC</t>
-  </si>
-  <si>
-    <t>UUUUG</t>
-  </si>
-  <si>
-    <t>UUUUU</t>
+    <t>AATAA</t>
+  </si>
+  <si>
+    <t>AATAC</t>
+  </si>
+  <si>
+    <t>AATAG</t>
+  </si>
+  <si>
+    <t>AATAT</t>
+  </si>
+  <si>
+    <t>AATCA</t>
+  </si>
+  <si>
+    <t>AATCC</t>
+  </si>
+  <si>
+    <t>AATCG</t>
+  </si>
+  <si>
+    <t>AATCT</t>
+  </si>
+  <si>
+    <t>AATGA</t>
+  </si>
+  <si>
+    <t>AATGC</t>
+  </si>
+  <si>
+    <t>AATGG</t>
+  </si>
+  <si>
+    <t>AATGT</t>
+  </si>
+  <si>
+    <t>AATTA</t>
+  </si>
+  <si>
+    <t>AATTC</t>
+  </si>
+  <si>
+    <t>AATTG</t>
+  </si>
+  <si>
+    <t>AATTT</t>
+  </si>
+  <si>
+    <t>ACTAA</t>
+  </si>
+  <si>
+    <t>ACTAC</t>
+  </si>
+  <si>
+    <t>ACTAG</t>
+  </si>
+  <si>
+    <t>ACTAT</t>
+  </si>
+  <si>
+    <t>ACTCA</t>
+  </si>
+  <si>
+    <t>ACTCC</t>
+  </si>
+  <si>
+    <t>ACTCG</t>
+  </si>
+  <si>
+    <t>ACTCT</t>
+  </si>
+  <si>
+    <t>ACTGA</t>
+  </si>
+  <si>
+    <t>ACTGC</t>
+  </si>
+  <si>
+    <t>ACTGG</t>
+  </si>
+  <si>
+    <t>ACTGT</t>
+  </si>
+  <si>
+    <t>ACTTA</t>
+  </si>
+  <si>
+    <t>ACTTC</t>
+  </si>
+  <si>
+    <t>ACTTG</t>
+  </si>
+  <si>
+    <t>ACTTT</t>
+  </si>
+  <si>
+    <t>AGTAA</t>
+  </si>
+  <si>
+    <t>AGTAC</t>
+  </si>
+  <si>
+    <t>AGTAG</t>
+  </si>
+  <si>
+    <t>AGTAT</t>
+  </si>
+  <si>
+    <t>AGTCA</t>
+  </si>
+  <si>
+    <t>AGTCC</t>
+  </si>
+  <si>
+    <t>AGTCG</t>
+  </si>
+  <si>
+    <t>AGTCT</t>
+  </si>
+  <si>
+    <t>AGTGA</t>
+  </si>
+  <si>
+    <t>AGTGC</t>
+  </si>
+  <si>
+    <t>AGTGG</t>
+  </si>
+  <si>
+    <t>AGTGT</t>
+  </si>
+  <si>
+    <t>AGTTA</t>
+  </si>
+  <si>
+    <t>AGTTC</t>
+  </si>
+  <si>
+    <t>AGTTG</t>
+  </si>
+  <si>
+    <t>AGTTT</t>
+  </si>
+  <si>
+    <t>ATTAA</t>
+  </si>
+  <si>
+    <t>ATTAC</t>
+  </si>
+  <si>
+    <t>ATTAG</t>
+  </si>
+  <si>
+    <t>ATTAT</t>
+  </si>
+  <si>
+    <t>ATTCA</t>
+  </si>
+  <si>
+    <t>ATTCC</t>
+  </si>
+  <si>
+    <t>ATTCG</t>
+  </si>
+  <si>
+    <t>ATTCT</t>
+  </si>
+  <si>
+    <t>ATTGA</t>
+  </si>
+  <si>
+    <t>ATTGC</t>
+  </si>
+  <si>
+    <t>ATTGG</t>
+  </si>
+  <si>
+    <t>ATTGT</t>
+  </si>
+  <si>
+    <t>ATTTA</t>
+  </si>
+  <si>
+    <t>ATTTC</t>
+  </si>
+  <si>
+    <t>ATTTG</t>
+  </si>
+  <si>
+    <t>ATTTT</t>
+  </si>
+  <si>
+    <t>CATAA</t>
+  </si>
+  <si>
+    <t>CATAC</t>
+  </si>
+  <si>
+    <t>CATAG</t>
+  </si>
+  <si>
+    <t>CATAT</t>
+  </si>
+  <si>
+    <t>CATCA</t>
+  </si>
+  <si>
+    <t>CATCC</t>
+  </si>
+  <si>
+    <t>CATCG</t>
+  </si>
+  <si>
+    <t>CATCT</t>
+  </si>
+  <si>
+    <t>CATGA</t>
+  </si>
+  <si>
+    <t>CATGC</t>
+  </si>
+  <si>
+    <t>CATGG</t>
+  </si>
+  <si>
+    <t>CATGT</t>
+  </si>
+  <si>
+    <t>CATTA</t>
+  </si>
+  <si>
+    <t>CATTC</t>
+  </si>
+  <si>
+    <t>CATTG</t>
+  </si>
+  <si>
+    <t>CATTT</t>
+  </si>
+  <si>
+    <t>CCTAA</t>
+  </si>
+  <si>
+    <t>CCTAC</t>
+  </si>
+  <si>
+    <t>CCTAG</t>
+  </si>
+  <si>
+    <t>CCTAT</t>
+  </si>
+  <si>
+    <t>CCTCA</t>
+  </si>
+  <si>
+    <t>CCTCC</t>
+  </si>
+  <si>
+    <t>CCTCG</t>
+  </si>
+  <si>
+    <t>CCTCT</t>
+  </si>
+  <si>
+    <t>CCTGA</t>
+  </si>
+  <si>
+    <t>CCTGC</t>
+  </si>
+  <si>
+    <t>CCTGG</t>
+  </si>
+  <si>
+    <t>CCTGT</t>
+  </si>
+  <si>
+    <t>CCTTA</t>
+  </si>
+  <si>
+    <t>CCTTC</t>
+  </si>
+  <si>
+    <t>CCTTG</t>
+  </si>
+  <si>
+    <t>CCTTT</t>
+  </si>
+  <si>
+    <t>CGTAA</t>
+  </si>
+  <si>
+    <t>CGTAC</t>
+  </si>
+  <si>
+    <t>CGTAG</t>
+  </si>
+  <si>
+    <t>CGTAT</t>
+  </si>
+  <si>
+    <t>CGTCA</t>
+  </si>
+  <si>
+    <t>CGTCC</t>
+  </si>
+  <si>
+    <t>CGTCG</t>
+  </si>
+  <si>
+    <t>CGTCT</t>
+  </si>
+  <si>
+    <t>CGTGA</t>
+  </si>
+  <si>
+    <t>CGTGC</t>
+  </si>
+  <si>
+    <t>CGTGG</t>
+  </si>
+  <si>
+    <t>CGTGT</t>
+  </si>
+  <si>
+    <t>CGTTA</t>
+  </si>
+  <si>
+    <t>CGTTC</t>
+  </si>
+  <si>
+    <t>CGTTG</t>
+  </si>
+  <si>
+    <t>CGTTT</t>
+  </si>
+  <si>
+    <t>CTTAA</t>
+  </si>
+  <si>
+    <t>CTTAC</t>
+  </si>
+  <si>
+    <t>CTTAG</t>
+  </si>
+  <si>
+    <t>CTTAT</t>
+  </si>
+  <si>
+    <t>CTTCA</t>
+  </si>
+  <si>
+    <t>CTTCC</t>
+  </si>
+  <si>
+    <t>CTTCG</t>
+  </si>
+  <si>
+    <t>CTTCT</t>
+  </si>
+  <si>
+    <t>CTTGA</t>
+  </si>
+  <si>
+    <t>CTTGC</t>
+  </si>
+  <si>
+    <t>CTTGG</t>
+  </si>
+  <si>
+    <t>CTTGT</t>
+  </si>
+  <si>
+    <t>CTTTA</t>
+  </si>
+  <si>
+    <t>CTTTC</t>
+  </si>
+  <si>
+    <t>CTTTG</t>
+  </si>
+  <si>
+    <t>CTTTT</t>
+  </si>
+  <si>
+    <t>GATAA</t>
+  </si>
+  <si>
+    <t>GATAC</t>
+  </si>
+  <si>
+    <t>GATAG</t>
+  </si>
+  <si>
+    <t>GATAT</t>
+  </si>
+  <si>
+    <t>GATCA</t>
+  </si>
+  <si>
+    <t>GATCC</t>
+  </si>
+  <si>
+    <t>GATCG</t>
+  </si>
+  <si>
+    <t>GATCT</t>
+  </si>
+  <si>
+    <t>GATGA</t>
+  </si>
+  <si>
+    <t>GATGC</t>
+  </si>
+  <si>
+    <t>GATGG</t>
+  </si>
+  <si>
+    <t>GATGT</t>
+  </si>
+  <si>
+    <t>GATTA</t>
+  </si>
+  <si>
+    <t>GATTC</t>
+  </si>
+  <si>
+    <t>GATTG</t>
+  </si>
+  <si>
+    <t>GATTT</t>
+  </si>
+  <si>
+    <t>GCTAA</t>
+  </si>
+  <si>
+    <t>GCTAC</t>
+  </si>
+  <si>
+    <t>GCTAG</t>
+  </si>
+  <si>
+    <t>GCTAT</t>
+  </si>
+  <si>
+    <t>GCTCA</t>
+  </si>
+  <si>
+    <t>GCTCC</t>
+  </si>
+  <si>
+    <t>GCTCG</t>
+  </si>
+  <si>
+    <t>GCTCT</t>
+  </si>
+  <si>
+    <t>GCTGA</t>
+  </si>
+  <si>
+    <t>GCTGC</t>
+  </si>
+  <si>
+    <t>GCTGG</t>
+  </si>
+  <si>
+    <t>GCTGT</t>
+  </si>
+  <si>
+    <t>GCTTA</t>
+  </si>
+  <si>
+    <t>GCTTC</t>
+  </si>
+  <si>
+    <t>GCTTG</t>
+  </si>
+  <si>
+    <t>GCTTT</t>
+  </si>
+  <si>
+    <t>GGTAA</t>
+  </si>
+  <si>
+    <t>GGTAC</t>
+  </si>
+  <si>
+    <t>GGTAG</t>
+  </si>
+  <si>
+    <t>GGTAT</t>
+  </si>
+  <si>
+    <t>GGTCA</t>
+  </si>
+  <si>
+    <t>GGTCC</t>
+  </si>
+  <si>
+    <t>GGTCG</t>
+  </si>
+  <si>
+    <t>GGTCT</t>
+  </si>
+  <si>
+    <t>GGTGA</t>
+  </si>
+  <si>
+    <t>GGTGC</t>
+  </si>
+  <si>
+    <t>GGTGG</t>
+  </si>
+  <si>
+    <t>GGTGT</t>
+  </si>
+  <si>
+    <t>GGTTA</t>
+  </si>
+  <si>
+    <t>GGTTC</t>
+  </si>
+  <si>
+    <t>GGTTG</t>
+  </si>
+  <si>
+    <t>GGTTT</t>
+  </si>
+  <si>
+    <t>GTTAA</t>
+  </si>
+  <si>
+    <t>GTTAC</t>
+  </si>
+  <si>
+    <t>GTTAG</t>
+  </si>
+  <si>
+    <t>GTTAT</t>
+  </si>
+  <si>
+    <t>GTTCA</t>
+  </si>
+  <si>
+    <t>GTTCC</t>
+  </si>
+  <si>
+    <t>GTTCG</t>
+  </si>
+  <si>
+    <t>GTTCT</t>
+  </si>
+  <si>
+    <t>GTTGA</t>
+  </si>
+  <si>
+    <t>GTTGC</t>
+  </si>
+  <si>
+    <t>GTTGG</t>
+  </si>
+  <si>
+    <t>GTTGT</t>
+  </si>
+  <si>
+    <t>GTTTA</t>
+  </si>
+  <si>
+    <t>GTTTC</t>
+  </si>
+  <si>
+    <t>GTTTG</t>
+  </si>
+  <si>
+    <t>GTTTT</t>
+  </si>
+  <si>
+    <t>TATAA</t>
+  </si>
+  <si>
+    <t>TATAC</t>
+  </si>
+  <si>
+    <t>TATAG</t>
+  </si>
+  <si>
+    <t>TATAT</t>
+  </si>
+  <si>
+    <t>TATCA</t>
+  </si>
+  <si>
+    <t>TATCC</t>
+  </si>
+  <si>
+    <t>TATCG</t>
+  </si>
+  <si>
+    <t>TATCT</t>
+  </si>
+  <si>
+    <t>TATGA</t>
+  </si>
+  <si>
+    <t>TATGC</t>
+  </si>
+  <si>
+    <t>TATGG</t>
+  </si>
+  <si>
+    <t>TATGT</t>
+  </si>
+  <si>
+    <t>TATTA</t>
+  </si>
+  <si>
+    <t>TATTC</t>
+  </si>
+  <si>
+    <t>TATTG</t>
+  </si>
+  <si>
+    <t>TATTT</t>
+  </si>
+  <si>
+    <t>TCTAA</t>
+  </si>
+  <si>
+    <t>TCTAC</t>
+  </si>
+  <si>
+    <t>TCTAG</t>
+  </si>
+  <si>
+    <t>TCTAT</t>
+  </si>
+  <si>
+    <t>TCTCA</t>
+  </si>
+  <si>
+    <t>TCTCC</t>
+  </si>
+  <si>
+    <t>TCTCG</t>
+  </si>
+  <si>
+    <t>TCTCT</t>
+  </si>
+  <si>
+    <t>TCTGA</t>
+  </si>
+  <si>
+    <t>TCTGC</t>
+  </si>
+  <si>
+    <t>TCTGG</t>
+  </si>
+  <si>
+    <t>TCTGT</t>
+  </si>
+  <si>
+    <t>TCTTA</t>
+  </si>
+  <si>
+    <t>TCTTC</t>
+  </si>
+  <si>
+    <t>TCTTG</t>
+  </si>
+  <si>
+    <t>TCTTT</t>
+  </si>
+  <si>
+    <t>TGTAA</t>
+  </si>
+  <si>
+    <t>TGTAC</t>
+  </si>
+  <si>
+    <t>TGTAG</t>
+  </si>
+  <si>
+    <t>TGTAT</t>
+  </si>
+  <si>
+    <t>TGTCA</t>
+  </si>
+  <si>
+    <t>TGTCC</t>
+  </si>
+  <si>
+    <t>TGTCG</t>
+  </si>
+  <si>
+    <t>TGTCT</t>
+  </si>
+  <si>
+    <t>TGTGA</t>
+  </si>
+  <si>
+    <t>TGTGC</t>
+  </si>
+  <si>
+    <t>TGTGG</t>
+  </si>
+  <si>
+    <t>TGTGT</t>
+  </si>
+  <si>
+    <t>TGTTA</t>
+  </si>
+  <si>
+    <t>TGTTC</t>
+  </si>
+  <si>
+    <t>TGTTG</t>
+  </si>
+  <si>
+    <t>TGTTT</t>
+  </si>
+  <si>
+    <t>TTTAA</t>
+  </si>
+  <si>
+    <t>TTTAC</t>
+  </si>
+  <si>
+    <t>TTTAG</t>
+  </si>
+  <si>
+    <t>TTTAT</t>
+  </si>
+  <si>
+    <t>TTTCA</t>
+  </si>
+  <si>
+    <t>TTTCC</t>
+  </si>
+  <si>
+    <t>TTTCG</t>
+  </si>
+  <si>
+    <t>TTTCT</t>
+  </si>
+  <si>
+    <t>TTTGA</t>
+  </si>
+  <si>
+    <t>TTTGC</t>
+  </si>
+  <si>
+    <t>TTTGG</t>
+  </si>
+  <si>
+    <t>TTTGT</t>
+  </si>
+  <si>
+    <t>TTTTA</t>
+  </si>
+  <si>
+    <t>TTTTC</t>
+  </si>
+  <si>
+    <t>TTTTG</t>
+  </si>
+  <si>
+    <t>TTTTT</t>
   </si>
 </sst>
 </file>
@@ -1219,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56FDA4D-0BD5-D64A-BED4-15600EC2EA01}">
   <dimension ref="A1:D257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="12.25"/>

</xml_diff>